<commit_message>
Completes Button-by-Button for current control system Updates gitignore for cerification and credential files
</commit_message>
<xml_diff>
--- a/Exhibit 27 40 00-11 Control System Button by Button.xlsx
+++ b/Exhibit 27 40 00-11 Control System Button by Button.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feuerhe1\Documents\Codespaces\UIUC_AV_StandardGUI_Extron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A9B0D7-D8C7-4B67-AE93-3D17E5EFC7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CBC5BB-3E07-4390-ABB1-9CEC19243540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="339">
   <si>
     <t>EXHIBIT 27 40 00-11, CONTROL SYSTEMS BUTTON BY BUTTON</t>
   </si>
@@ -723,6 +723,336 @@
   </si>
   <si>
     <t>Toggles panel wake on motion</t>
+  </si>
+  <si>
+    <t>Camera Select</t>
+  </si>
+  <si>
+    <t>Selects which camera the rest of the controls operate</t>
+  </si>
+  <si>
+    <t>Only shown if more than 1 camera in the system</t>
+  </si>
+  <si>
+    <t>Preset Select (Press)</t>
+  </si>
+  <si>
+    <t>Preset Select (Held)</t>
+  </si>
+  <si>
+    <t>Opens Camera Preset Editor popup page</t>
+  </si>
+  <si>
+    <t>Pan/Tilt Arrows (Press)</t>
+  </si>
+  <si>
+    <t>Starts Pan/Tilt action</t>
+  </si>
+  <si>
+    <t>Pan/Tilt Arrows (Release)</t>
+  </si>
+  <si>
+    <t>Stops Pan/Tilt action</t>
+  </si>
+  <si>
+    <t>Zoom Buttons (Press)</t>
+  </si>
+  <si>
+    <t>Starts Zoom action</t>
+  </si>
+  <si>
+    <t>Zoom Buttons (Release)</t>
+  </si>
+  <si>
+    <t>Stops Zoom action</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Sends Camera to Home location</t>
+  </si>
+  <si>
+    <t>Sends camera to selected preset location</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>None implemented at this time</t>
+  </si>
+  <si>
+    <t>All Mics Toggle</t>
+  </si>
+  <si>
+    <t>1 per mic channel</t>
+  </si>
+  <si>
+    <t>Toggles mic mute</t>
+  </si>
+  <si>
+    <t>Mic Vol Up (Press)</t>
+  </si>
+  <si>
+    <t>Mic Vol Up (Hold)</t>
+  </si>
+  <si>
+    <t>Mic Vol Down (Press)</t>
+  </si>
+  <si>
+    <t>MIc Vol Down (Hold)</t>
+  </si>
+  <si>
+    <t>Nudges mic volume up</t>
+  </si>
+  <si>
+    <t>Shifts mic volume up while held</t>
+  </si>
+  <si>
+    <t>Nudges mic volume down</t>
+  </si>
+  <si>
+    <t>Shifts mic volume down while held</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Closes popover</t>
+  </si>
+  <si>
+    <t>Closes destination popup</t>
+  </si>
+  <si>
+    <t>Gain Up</t>
+  </si>
+  <si>
+    <t>Gain Down</t>
+  </si>
+  <si>
+    <t>Phantom Power Toggle</t>
+  </si>
+  <si>
+    <t>Nudges channel gain up</t>
+  </si>
+  <si>
+    <t>Nudges channel gain down</t>
+  </si>
+  <si>
+    <t>Toggles phantom power</t>
+  </si>
+  <si>
+    <t>1 per input channel</t>
+  </si>
+  <si>
+    <t>Displays next page of input channel configuration objects</t>
+  </si>
+  <si>
+    <t>Displays previous page of input channel configuration objects</t>
+  </si>
+  <si>
+    <t>Auto Start toggle</t>
+  </si>
+  <si>
+    <t>Start Schedule button</t>
+  </si>
+  <si>
+    <t>Start Activity buttons</t>
+  </si>
+  <si>
+    <t>1 per activity</t>
+  </si>
+  <si>
+    <t>Toggles automatic system startup based on configured schedule</t>
+  </si>
+  <si>
+    <t>Selects activity for Start Schedule to start system into</t>
+  </si>
+  <si>
+    <t>Auto Shutdown toggle</t>
+  </si>
+  <si>
+    <t>Toggles automatic system shutdown based on configured schedule</t>
+  </si>
+  <si>
+    <t>Shutdown Schedule button</t>
+  </si>
+  <si>
+    <t>Opens Schedule Editor Popup for Start Schedule</t>
+  </si>
+  <si>
+    <t>Opens Schedule Editor Popup for Shutdown Schedule</t>
+  </si>
+  <si>
+    <t>Show Tips</t>
+  </si>
+  <si>
+    <t>Shows dismissable user tip for 60 seconds before automatically dismissing tip and showing selected source controls</t>
+  </si>
+  <si>
+    <t>Clear Posts</t>
+  </si>
+  <si>
+    <t>Clear Posts &amp; Users</t>
+  </si>
+  <si>
+    <t>Clears posts from selected Mersive Solstice device</t>
+  </si>
+  <si>
+    <t>Clears posts and users from select Mersive Solstice device</t>
+  </si>
+  <si>
+    <t>Screen Up</t>
+  </si>
+  <si>
+    <t>Screen Down</t>
+  </si>
+  <si>
+    <t>Screen Stop</t>
+  </si>
+  <si>
+    <t>Preset Name</t>
+  </si>
+  <si>
+    <t>Reset to Home Position</t>
+  </si>
+  <si>
+    <t>Save Preset</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Closes Camera Preset Editor and saves changes</t>
+  </si>
+  <si>
+    <t>Closes Camera Preset Editor without saving changes</t>
+  </si>
+  <si>
+    <t>Sends camera to home Position</t>
+  </si>
+  <si>
+    <t>Opens keyboard</t>
+  </si>
+  <si>
+    <t>Day-of-Week Buttons (Monday - Sunday)</t>
+  </si>
+  <si>
+    <t>Toggles day for schedule configuration</t>
+  </si>
+  <si>
+    <t>Select All Days</t>
+  </si>
+  <si>
+    <t>Selects all days for schedule configuration</t>
+  </si>
+  <si>
+    <t>Selects Weekdays</t>
+  </si>
+  <si>
+    <t>Selects only Monday through Friday for schedule configuration</t>
+  </si>
+  <si>
+    <t>Hour Arrows</t>
+  </si>
+  <si>
+    <t>Minute Arrows</t>
+  </si>
+  <si>
+    <t>Increases/Decreases hour by one (13 rolls over to 1, 0 rolls over to 12)</t>
+  </si>
+  <si>
+    <t>Increases/Decreases minute by one (60 rolls over to 0, -1 rolls over to 59)</t>
+  </si>
+  <si>
+    <t>AM/PM Buttons</t>
+  </si>
+  <si>
+    <t>Selects AM/PM for schedule configuration time</t>
+  </si>
+  <si>
+    <t>Save Schedule</t>
+  </si>
+  <si>
+    <t>Closes Schedule Editor Popup and saves schedule configuration changes</t>
+  </si>
+  <si>
+    <t>Closes Schedule Editor Popup without saving schedule changes</t>
+  </si>
+  <si>
+    <t>Character Keys</t>
+  </si>
+  <si>
+    <t>Inserts character at cursor position</t>
+  </si>
+  <si>
+    <t>Del</t>
+  </si>
+  <si>
+    <t>Deletes character after cursor</t>
+  </si>
+  <si>
+    <t>Backspace</t>
+  </si>
+  <si>
+    <t>Deletes character before cursor</t>
+  </si>
+  <si>
+    <t>Toggles capital letters and special characters</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Toggles capital letters and special characters for the next input</t>
+  </si>
+  <si>
+    <t>Caps Lock</t>
+  </si>
+  <si>
+    <t>Caps Lock and shift keys cancel each other out</t>
+  </si>
+  <si>
+    <t>Cursor Left/Right</t>
+  </si>
+  <si>
+    <t>Shifts cursor one character to the Left/Right</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Closes keyboard popup and saves new text string</t>
+  </si>
+  <si>
+    <t>Closes keyboard popup without saving next text string</t>
+  </si>
+  <si>
+    <t>Numeral buttons</t>
+  </si>
+  <si>
+    <t>Inserts the selected numeral into the PIN string for verification</t>
+  </si>
+  <si>
+    <t>Removes the last entered character from the PIN string</t>
+  </si>
+  <si>
+    <t>Clears the pin data</t>
+  </si>
+  <si>
+    <t>Closes the PIN Entry Popup</t>
+  </si>
+  <si>
+    <t>Ends shutdown timer</t>
+  </si>
+  <si>
+    <t>Returns to Main page configured to the current activity</t>
+  </si>
+  <si>
+    <t>End Now</t>
+  </si>
+  <si>
+    <t>Begins shutting system down immediately</t>
   </si>
 </sst>
 </file>
@@ -766,7 +1096,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,12 +1110,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -808,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,11 +1183,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1176,15 +1496,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D545"/>
+  <dimension ref="A1:D856"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D509" sqref="D509"/>
+    <sheetView tabSelected="1" topLeftCell="A845" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D856" sqref="D856"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" style="14" customWidth="1"/>
     <col min="2" max="2" width="1.85546875" customWidth="1"/>
     <col min="3" max="3" width="59.140625" customWidth="1"/>
     <col min="4" max="4" width="78.28515625" customWidth="1"/>
@@ -2068,7 +2388,7 @@
       <c r="A113" s="12"/>
       <c r="B113" s="1"/>
       <c r="C113" s="12"/>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3388,7 +3708,7 @@
     <row r="287" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="12"/>
       <c r="B287" s="15"/>
-      <c r="C287" s="26" t="s">
+      <c r="C287" s="23" t="s">
         <v>151</v>
       </c>
       <c r="D287" s="21" t="s">
@@ -3398,7 +3718,7 @@
     <row r="288" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" s="12"/>
       <c r="B288" s="15"/>
-      <c r="C288" s="26"/>
+      <c r="C288" s="23"/>
       <c r="D288" s="7" t="s">
         <v>165</v>
       </c>
@@ -3406,13 +3726,13 @@
     <row r="289" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" s="12"/>
       <c r="B289" s="15"/>
-      <c r="C289" s="26"/>
+      <c r="C289" s="23"/>
       <c r="D289" s="15"/>
     </row>
     <row r="290" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="12"/>
       <c r="B290" s="15"/>
-      <c r="C290" s="26" t="s">
+      <c r="C290" s="23" t="s">
         <v>152</v>
       </c>
       <c r="D290" s="21" t="s">
@@ -3422,7 +3742,7 @@
     <row r="291" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="12"/>
       <c r="B291" s="15"/>
-      <c r="C291" s="26"/>
+      <c r="C291" s="23"/>
       <c r="D291" s="7" t="s">
         <v>168</v>
       </c>
@@ -3430,13 +3750,13 @@
     <row r="292" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="12"/>
       <c r="B292" s="15"/>
-      <c r="C292" s="26"/>
+      <c r="C292" s="23"/>
       <c r="D292" s="15"/>
     </row>
     <row r="293" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="12"/>
       <c r="B293" s="15"/>
-      <c r="C293" s="26" t="s">
+      <c r="C293" s="23" t="s">
         <v>153</v>
       </c>
       <c r="D293" s="21" t="s">
@@ -3446,7 +3766,7 @@
     <row r="294" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="12"/>
       <c r="B294" s="15"/>
-      <c r="C294" s="26"/>
+      <c r="C294" s="23"/>
       <c r="D294" s="7" t="s">
         <v>170</v>
       </c>
@@ -3454,13 +3774,13 @@
     <row r="295" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="12"/>
       <c r="B295" s="15"/>
-      <c r="C295" s="26"/>
+      <c r="C295" s="23"/>
       <c r="D295" s="15"/>
     </row>
     <row r="296" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="12"/>
       <c r="B296" s="15"/>
-      <c r="C296" s="26" t="s">
+      <c r="C296" s="23" t="s">
         <v>154</v>
       </c>
       <c r="D296" s="15"/>
@@ -3468,7 +3788,7 @@
     <row r="297" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="12"/>
       <c r="B297" s="15"/>
-      <c r="C297" s="26"/>
+      <c r="C297" s="23"/>
       <c r="D297" s="7" t="s">
         <v>171</v>
       </c>
@@ -3476,12 +3796,12 @@
     <row r="298" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="12"/>
       <c r="B298" s="15"/>
-      <c r="C298" s="26"/>
+      <c r="C298" s="23"/>
     </row>
     <row r="299" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="12"/>
       <c r="B299" s="15"/>
-      <c r="C299" s="26" t="s">
+      <c r="C299" s="23" t="s">
         <v>155</v>
       </c>
       <c r="D299" s="15"/>
@@ -3489,7 +3809,7 @@
     <row r="300" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="12"/>
       <c r="B300" s="15"/>
-      <c r="C300" s="26"/>
+      <c r="C300" s="23"/>
       <c r="D300" s="7" t="s">
         <v>172</v>
       </c>
@@ -4304,387 +4624,378 @@
       </c>
     </row>
     <row r="415" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A415" s="29" t="s">
+      <c r="A415" s="26" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="416" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A416" s="29"/>
+      <c r="A416" s="26"/>
       <c r="C416" s="8" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="417" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A417" s="29"/>
+      <c r="A417" s="26"/>
       <c r="D417" s="8" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A418" s="29"/>
+      <c r="A418" s="26"/>
       <c r="C418" s="8" t="s">
         <v>129</v>
       </c>
       <c r="D418" s="8"/>
     </row>
     <row r="419" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A419" s="29"/>
+      <c r="A419" s="26"/>
       <c r="D419" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="420" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A420" s="28"/>
-    </row>
     <row r="421" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A421" s="29" t="s">
+      <c r="A421" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="422" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A422" s="29"/>
+      <c r="A422" s="26"/>
       <c r="C422" s="8" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A423" s="29"/>
+      <c r="A423" s="26"/>
       <c r="C423" s="8"/>
       <c r="D423" s="8" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A424" s="29"/>
+      <c r="A424" s="26"/>
       <c r="C424" s="8"/>
     </row>
     <row r="425" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A425" s="29"/>
+      <c r="A425" s="26"/>
       <c r="C425" s="8" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="426" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A426" s="29"/>
+      <c r="A426" s="26"/>
       <c r="C426" s="8"/>
       <c r="D426" s="8" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="427" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A427" s="29"/>
+      <c r="A427" s="26"/>
       <c r="C427" s="8"/>
     </row>
     <row r="428" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A428" s="29"/>
+      <c r="A428" s="26"/>
       <c r="C428" s="8" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A429" s="29"/>
+      <c r="A429" s="26"/>
       <c r="C429" s="8"/>
       <c r="D429" s="8" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A430" s="29"/>
+      <c r="A430" s="26"/>
       <c r="C430" s="8"/>
     </row>
     <row r="431" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A431" s="29"/>
+      <c r="A431" s="26"/>
       <c r="C431" s="8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="432" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A432" s="29"/>
+      <c r="A432" s="26"/>
       <c r="C432" s="8"/>
       <c r="D432" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="433" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A433" s="29"/>
+      <c r="A433" s="26"/>
       <c r="C433" s="8"/>
     </row>
     <row r="434" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A434" s="29"/>
+      <c r="A434" s="26"/>
       <c r="C434" s="8" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="435" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A435" s="29"/>
+      <c r="A435" s="26"/>
       <c r="C435" s="8"/>
       <c r="D435" s="8" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="436" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A436" s="29"/>
+      <c r="A436" s="26"/>
       <c r="C436" s="8"/>
     </row>
     <row r="437" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A437" s="29"/>
+      <c r="A437" s="26"/>
       <c r="C437" s="8" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="438" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A438" s="29"/>
+      <c r="A438" s="26"/>
       <c r="C438" s="8"/>
       <c r="D438" s="8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="439" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A439" s="29"/>
+      <c r="A439" s="26"/>
       <c r="C439" s="8"/>
     </row>
     <row r="440" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A440" s="29"/>
+      <c r="A440" s="26"/>
       <c r="C440" s="8" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="441" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A441" s="29"/>
+      <c r="A441" s="26"/>
       <c r="C441" s="8"/>
       <c r="D441" s="8" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A442" s="29"/>
+      <c r="A442" s="26"/>
       <c r="C442" s="8"/>
     </row>
     <row r="443" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A443" s="29"/>
+      <c r="A443" s="26"/>
       <c r="C443" s="8" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="444" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A444" s="29"/>
+      <c r="A444" s="26"/>
       <c r="C444" s="8"/>
       <c r="D444" s="8" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A445" s="29"/>
+      <c r="A445" s="26"/>
       <c r="C445" s="8"/>
     </row>
     <row r="446" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A446" s="29"/>
+      <c r="A446" s="26"/>
       <c r="C446" s="8" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="447" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A447" s="29"/>
+      <c r="A447" s="26"/>
       <c r="C447" s="8"/>
       <c r="D447" s="8" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="448" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A448" s="29"/>
+      <c r="A448" s="26"/>
       <c r="C448" s="8"/>
     </row>
     <row r="449" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A449" s="29"/>
+      <c r="A449" s="26"/>
       <c r="C449" s="8" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="450" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A450" s="29"/>
+      <c r="A450" s="26"/>
       <c r="C450" s="8"/>
       <c r="D450" s="8" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A451" s="29"/>
+      <c r="A451" s="26"/>
       <c r="C451" s="8"/>
     </row>
     <row r="452" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A452" s="29"/>
+      <c r="A452" s="26"/>
       <c r="C452" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="453" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A453" s="29"/>
+      <c r="A453" s="26"/>
       <c r="C453" s="8"/>
       <c r="D453" s="8" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="454" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A454" s="29"/>
+      <c r="A454" s="26"/>
       <c r="C454" s="8"/>
     </row>
     <row r="455" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A455" s="29"/>
+      <c r="A455" s="26"/>
       <c r="C455" s="8" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="456" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A456" s="29"/>
+      <c r="A456" s="26"/>
       <c r="C456" s="8"/>
       <c r="D456" s="8" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="457" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A457" s="29"/>
+      <c r="A457" s="26"/>
       <c r="C457" s="8"/>
     </row>
     <row r="458" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A458" s="29"/>
+      <c r="A458" s="26"/>
       <c r="C458" s="8" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="459" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A459" s="29"/>
+      <c r="A459" s="26"/>
       <c r="C459" s="8"/>
       <c r="D459" s="8" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="460" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A460" s="29"/>
+      <c r="A460" s="26"/>
       <c r="C460" s="8"/>
     </row>
     <row r="461" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A461" s="29"/>
+      <c r="A461" s="26"/>
       <c r="C461" s="8" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="462" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A462" s="29"/>
+      <c r="A462" s="26"/>
       <c r="C462" s="8"/>
       <c r="D462" s="8" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="463" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A463" s="29"/>
-    </row>
-    <row r="464" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A464" s="28"/>
+      <c r="A463" s="26"/>
     </row>
     <row r="465" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A465" s="29" t="s">
+      <c r="A465" s="26" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="466" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A466" s="29"/>
+      <c r="A466" s="26"/>
       <c r="C466" s="8" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="467" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A467" s="29"/>
+      <c r="A467" s="26"/>
       <c r="C467" s="8"/>
       <c r="D467" s="8" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="468" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A468" s="29"/>
+      <c r="A468" s="26"/>
       <c r="C468" s="8"/>
     </row>
     <row r="469" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A469" s="29"/>
+      <c r="A469" s="26"/>
       <c r="C469" s="8" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="470" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A470" s="29"/>
+      <c r="A470" s="26"/>
       <c r="C470" s="8"/>
       <c r="D470" s="8" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="471" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A471" s="29"/>
+      <c r="A471" s="26"/>
       <c r="C471" s="8"/>
     </row>
     <row r="472" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A472" s="29"/>
+      <c r="A472" s="26"/>
       <c r="C472" s="8" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="473" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A473" s="29"/>
+      <c r="A473" s="26"/>
       <c r="C473" s="8"/>
       <c r="D473" s="8" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="474" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A474" s="29"/>
+      <c r="A474" s="26"/>
       <c r="C474" s="8"/>
     </row>
     <row r="475" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A475" s="29"/>
+      <c r="A475" s="26"/>
       <c r="C475" s="8" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="476" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A476" s="29"/>
+      <c r="A476" s="26"/>
       <c r="C476" s="8"/>
       <c r="D476" s="8" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="477" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A477" s="29"/>
+      <c r="A477" s="26"/>
       <c r="C477" s="8"/>
     </row>
     <row r="478" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A478" s="29"/>
+      <c r="A478" s="26"/>
       <c r="C478" s="8" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="479" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A479" s="29"/>
+      <c r="A479" s="26"/>
       <c r="C479" s="8"/>
       <c r="D479" s="8" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="480" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A480" s="29"/>
+      <c r="A480" s="26"/>
       <c r="C480" s="8"/>
     </row>
     <row r="481" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A481" s="29"/>
+      <c r="A481" s="26"/>
       <c r="C481" s="8" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="482" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A482" s="29"/>
+      <c r="A482" s="26"/>
       <c r="D482" s="8" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="483" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A483" s="28"/>
     </row>
     <row r="484" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A484" s="27" t="s">
@@ -4692,278 +5003,2004 @@
       </c>
     </row>
     <row r="485" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A485" s="28"/>
+      <c r="A485" s="27"/>
+      <c r="C485" t="s">
+        <v>229</v>
+      </c>
+      <c r="D485" s="25" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="486" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A486" s="27" t="s">
+      <c r="A486" s="27"/>
+      <c r="D486" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A487" s="27"/>
+    </row>
+    <row r="488" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A488" s="27"/>
+      <c r="C488" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A489" s="27"/>
+      <c r="D489" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A490" s="27"/>
+    </row>
+    <row r="491" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A491" s="27"/>
+      <c r="C491" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A492" s="27"/>
+      <c r="D492" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A493" s="27"/>
+    </row>
+    <row r="494" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A494" s="27"/>
+      <c r="C494" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A495" s="27"/>
+      <c r="D495" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A496" s="27"/>
+    </row>
+    <row r="497" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A497" s="27"/>
+      <c r="C497" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A498" s="27"/>
+      <c r="D498" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A499" s="27"/>
+    </row>
+    <row r="500" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A500" s="27"/>
+      <c r="C500" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="27"/>
+      <c r="D501" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="27"/>
+    </row>
+    <row r="503" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="27"/>
+      <c r="C503" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A504" s="27"/>
+      <c r="D504" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="27"/>
+    </row>
+    <row r="506" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A506" s="27"/>
+      <c r="C506" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A507" s="27"/>
+      <c r="D507" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="27" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="487" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A487" s="28"/>
-    </row>
-    <row r="488" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A488" s="27" t="s">
+    <row r="510" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="27"/>
+      <c r="C510" t="s">
+        <v>262</v>
+      </c>
+      <c r="D510" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="27"/>
+      <c r="D511" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="27"/>
+    </row>
+    <row r="513" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A513" s="27"/>
+      <c r="C513" t="s">
+        <v>263</v>
+      </c>
+      <c r="D513" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A514" s="27"/>
+      <c r="D514" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A515" s="27"/>
+    </row>
+    <row r="516" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A516" s="27"/>
+      <c r="C516" t="s">
+        <v>264</v>
+      </c>
+      <c r="D516" s="25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A517" s="27"/>
+      <c r="D517" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A518" s="27"/>
+    </row>
+    <row r="519" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A519" s="27"/>
+      <c r="C519" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A520" s="27"/>
+      <c r="D520" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A521" s="27"/>
+    </row>
+    <row r="522" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A522" s="27"/>
+      <c r="C522" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="523" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A523" s="27"/>
+      <c r="D523" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="525" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A525" s="27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="526" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A526" s="27"/>
+      <c r="C526" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="527" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A527" s="27"/>
+      <c r="D527" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="528" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A528" s="27"/>
+    </row>
+    <row r="529" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A529" s="27"/>
+      <c r="C529" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A530" s="27"/>
+      <c r="D530" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A531" s="27"/>
+    </row>
+    <row r="532" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A532" s="27"/>
+      <c r="C532" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D532" s="25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A533" s="27"/>
+      <c r="D533" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A534" s="27"/>
+    </row>
+    <row r="535" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A535" s="27"/>
+      <c r="C535" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A536" s="27"/>
+      <c r="D536" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A537" s="27"/>
+    </row>
+    <row r="538" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A538" s="27"/>
+      <c r="C538" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A539" s="27"/>
+      <c r="D539" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A541" s="27" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="489" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A489" s="28"/>
-    </row>
-    <row r="490" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A490" s="27" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="491" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A491" s="28"/>
-    </row>
-    <row r="492" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A492" s="27" t="s">
+    <row r="542" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A542" s="27"/>
+      <c r="C542" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D542" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A544" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="493" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A493" s="28"/>
-    </row>
-    <row r="494" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A494" s="29" t="s">
+    <row r="545" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A545" s="12"/>
+      <c r="B545" s="1"/>
+      <c r="C545" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D545" s="7"/>
+    </row>
+    <row r="546" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A546" s="12"/>
+      <c r="B546" s="1"/>
+      <c r="C546" s="12"/>
+      <c r="D546" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A547" s="12"/>
+      <c r="B547" s="1"/>
+      <c r="C547" s="12"/>
+      <c r="D547" s="7"/>
+    </row>
+    <row r="548" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A548" s="12"/>
+      <c r="B548" s="1"/>
+      <c r="C548" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D548" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A549" s="12"/>
+      <c r="B549" s="1"/>
+      <c r="C549" s="12"/>
+      <c r="D549" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A550" s="12"/>
+      <c r="B550" s="1"/>
+      <c r="C550" s="12"/>
+      <c r="D550" s="7"/>
+    </row>
+    <row r="551" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A551" s="12"/>
+      <c r="B551" s="1"/>
+      <c r="C551" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D551" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A552" s="12"/>
+      <c r="B552" s="1"/>
+      <c r="C552" s="12"/>
+      <c r="D552" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A553" s="12"/>
+      <c r="B553" s="1"/>
+      <c r="C553" s="12"/>
+      <c r="D553" s="7"/>
+    </row>
+    <row r="554" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A554" s="12"/>
+      <c r="B554" s="1"/>
+      <c r="C554" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D554" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A555" s="12"/>
+      <c r="B555" s="1"/>
+      <c r="C555" s="12"/>
+      <c r="D555" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A556" s="12"/>
+      <c r="B556" s="1"/>
+      <c r="C556" s="12"/>
+      <c r="D556" s="20"/>
+    </row>
+    <row r="557" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A557" s="12"/>
+      <c r="B557" s="15"/>
+      <c r="C557" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D557" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A558" s="12"/>
+      <c r="B558" s="15"/>
+      <c r="C558" s="15"/>
+      <c r="D558" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A559" s="12"/>
+      <c r="B559" s="15"/>
+      <c r="C559" s="15"/>
+      <c r="D559" s="7"/>
+    </row>
+    <row r="560" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A560" s="12"/>
+      <c r="B560" s="1"/>
+      <c r="C560" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D560" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A561" s="12"/>
+      <c r="B561" s="1"/>
+      <c r="C561" s="12"/>
+      <c r="D561" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A562" s="12"/>
+      <c r="B562" s="1"/>
+      <c r="C562" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D562" s="6"/>
+    </row>
+    <row r="563" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A563" s="12"/>
+      <c r="B563" s="1"/>
+      <c r="C563" s="12"/>
+      <c r="D563" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A564" s="12"/>
+      <c r="B564" s="1"/>
+      <c r="C564" s="12"/>
+      <c r="D564" s="7"/>
+    </row>
+    <row r="565" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A565" s="12"/>
+      <c r="B565" s="1"/>
+      <c r="C565" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D565" s="7"/>
+    </row>
+    <row r="566" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A566" s="12"/>
+      <c r="B566" s="1"/>
+      <c r="C566" s="12"/>
+      <c r="D566" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A567" s="12"/>
+      <c r="B567" s="1"/>
+      <c r="C567" s="12"/>
+      <c r="D567" s="7"/>
+    </row>
+    <row r="568" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A568" s="12"/>
+      <c r="B568" s="1"/>
+      <c r="C568" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D568" s="10"/>
+    </row>
+    <row r="569" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A569" s="12"/>
+      <c r="B569" s="1"/>
+      <c r="C569" s="12"/>
+      <c r="D569" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A570" s="12"/>
+      <c r="B570" s="1"/>
+      <c r="C570" s="12"/>
+      <c r="D570" s="20"/>
+    </row>
+    <row r="571" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A571" s="12"/>
+      <c r="B571" s="15"/>
+      <c r="C571" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D571" s="6"/>
+    </row>
+    <row r="572" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A572" s="12"/>
+      <c r="B572" s="15"/>
+      <c r="C572" s="15"/>
+      <c r="D572" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A573" s="12"/>
+      <c r="B573" s="15"/>
+      <c r="C573" s="15"/>
+      <c r="D573" s="7"/>
+    </row>
+    <row r="574" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A574" s="12"/>
+      <c r="B574" s="1"/>
+      <c r="C574" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D574" s="10"/>
+    </row>
+    <row r="575" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A575" s="12"/>
+      <c r="B575" s="1"/>
+      <c r="C575" s="12"/>
+      <c r="D575" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A577" s="26" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="495" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A495" s="29"/>
-      <c r="C495" s="8" t="s">
+    <row r="578" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A578" s="26"/>
+      <c r="C578" s="8" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="496" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A496" s="29"/>
-      <c r="C496" s="8"/>
-      <c r="D496" s="8" t="s">
+    <row r="579" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A579" s="26"/>
+      <c r="C579" s="8"/>
+      <c r="D579" s="8" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="497" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A497" s="29"/>
-    </row>
-    <row r="498" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A498" s="29"/>
-      <c r="C498" s="8" t="s">
+    <row r="580" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A580" s="26"/>
+    </row>
+    <row r="581" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A581" s="26"/>
+      <c r="C581" s="8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="499" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A499" s="29"/>
-      <c r="C499" s="8"/>
-      <c r="D499" s="8" t="s">
+    <row r="582" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A582" s="26"/>
+      <c r="C582" s="8"/>
+      <c r="D582" s="8" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="500" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A500" s="29"/>
-    </row>
-    <row r="501" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A501" s="29"/>
-      <c r="C501" s="8" t="s">
+    <row r="583" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A583" s="26"/>
+    </row>
+    <row r="584" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A584" s="26"/>
+      <c r="C584" s="8" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="502" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A502" s="29"/>
-      <c r="C502" s="8"/>
-      <c r="D502" s="8" t="s">
+    <row r="585" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A585" s="26"/>
+      <c r="C585" s="8"/>
+      <c r="D585" s="8" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="503" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A503" s="29"/>
-      <c r="C503" s="8" t="s">
+    <row r="586" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A586" s="26"/>
+      <c r="C586" s="8"/>
+    </row>
+    <row r="587" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A587" s="26"/>
+      <c r="C587" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A588" s="26"/>
+      <c r="C588" s="8"/>
+      <c r="D588" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A589" s="26"/>
+    </row>
+    <row r="590" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A590" s="26"/>
+      <c r="C590" s="8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A591" s="26"/>
+      <c r="C591" s="8"/>
+      <c r="D591" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A592" s="26"/>
+    </row>
+    <row r="593" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A593" s="26"/>
+      <c r="C593" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A594" s="26"/>
+      <c r="C594" s="8"/>
+      <c r="D594" s="8" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="504" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A504" s="29"/>
-      <c r="C504" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="505" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A505" s="29"/>
-      <c r="C505" s="8"/>
-      <c r="D505" s="8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="506" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A506" s="29"/>
-    </row>
-    <row r="507" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A507" s="29"/>
-      <c r="C507" s="8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="508" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A508" s="29"/>
-      <c r="C508" s="8"/>
-      <c r="D508" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="509" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A509" s="29"/>
-    </row>
-    <row r="510" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A510" s="29"/>
-      <c r="C510" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="511" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A511" s="29"/>
-      <c r="C511" s="8"/>
-      <c r="D511" s="8" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="512" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A512" s="28"/>
-    </row>
-    <row r="513" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A513" s="29" t="s">
+    <row r="596" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A596" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C513" s="25" t="s">
+      <c r="C596" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="514" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A514" s="28"/>
-    </row>
-    <row r="515" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A515" s="27" t="s">
+    <row r="598" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A598" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="516" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A516" s="28"/>
-    </row>
-    <row r="517" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A517" s="27" t="s">
+    <row r="599" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A599" s="27"/>
+      <c r="C599" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A600" s="27"/>
+      <c r="D600" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A602" s="27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="518" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A518" s="28"/>
-    </row>
-    <row r="519" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A519" s="27" t="s">
+    <row r="603" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A603" s="27"/>
+      <c r="C603" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A604" s="27"/>
+      <c r="D604" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A605" s="27"/>
+      <c r="D605" s="8"/>
+    </row>
+    <row r="606" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A606" s="27"/>
+      <c r="C606" t="s">
+        <v>229</v>
+      </c>
+      <c r="D606" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A607" s="27"/>
+      <c r="D607" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A608" s="27"/>
+    </row>
+    <row r="609" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A609" s="27"/>
+      <c r="C609" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A610" s="27"/>
+      <c r="D610" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A611" s="27"/>
+    </row>
+    <row r="612" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A612" s="27"/>
+      <c r="C612" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A613" s="27"/>
+      <c r="D613" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A614" s="27"/>
+    </row>
+    <row r="615" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A615" s="27"/>
+      <c r="C615" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A616" s="27"/>
+      <c r="D616" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A617" s="27"/>
+    </row>
+    <row r="618" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A618" s="27"/>
+      <c r="C618" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A619" s="27"/>
+      <c r="D619" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A620" s="27"/>
+    </row>
+    <row r="621" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A621" s="27"/>
+      <c r="C621" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A622" s="27"/>
+      <c r="D622" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A623" s="27"/>
+    </row>
+    <row r="624" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A624" s="27"/>
+      <c r="C624" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A625" s="27"/>
+      <c r="D625" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A627" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="520" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A520" s="28"/>
-    </row>
-    <row r="521" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A521" s="27" t="s">
+    <row r="628" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A628" s="27"/>
+      <c r="C628" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A629" s="27"/>
+      <c r="D629" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A631" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="522" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A522" s="28"/>
-    </row>
-    <row r="523" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A523" s="27" t="s">
+    <row r="632" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A632" s="27"/>
+      <c r="C632" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A633" s="27"/>
+      <c r="D633" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A635" s="12"/>
+      <c r="B635" s="1"/>
+      <c r="C635" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="D635" s="7"/>
+    </row>
+    <row r="636" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A636" s="12"/>
+      <c r="B636" s="1"/>
+      <c r="C636" s="12"/>
+      <c r="D636" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A637" s="12"/>
+      <c r="B637" s="1"/>
+      <c r="C637" s="12"/>
+      <c r="D637" s="7"/>
+    </row>
+    <row r="638" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A638" s="12"/>
+      <c r="B638" s="1"/>
+      <c r="C638" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D638" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A639" s="12"/>
+      <c r="B639" s="1"/>
+      <c r="C639" s="12"/>
+      <c r="D639" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A640" s="12"/>
+      <c r="B640" s="1"/>
+      <c r="C640" s="12"/>
+      <c r="D640" s="7"/>
+    </row>
+    <row r="641" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A641" s="12"/>
+      <c r="B641" s="1"/>
+      <c r="C641" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D641" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A642" s="12"/>
+      <c r="B642" s="1"/>
+      <c r="C642" s="12"/>
+      <c r="D642" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A643" s="12"/>
+      <c r="B643" s="1"/>
+      <c r="C643" s="12"/>
+      <c r="D643" s="7"/>
+    </row>
+    <row r="644" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A644" s="12"/>
+      <c r="B644" s="1"/>
+      <c r="C644" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D644" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A645" s="12"/>
+      <c r="B645" s="1"/>
+      <c r="C645" s="12"/>
+      <c r="D645" s="10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="646" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A646" s="12"/>
+      <c r="B646" s="1"/>
+      <c r="C646" s="12"/>
+      <c r="D646" s="20"/>
+    </row>
+    <row r="647" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A647" s="12"/>
+      <c r="B647" s="15"/>
+      <c r="C647" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D647" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="648" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A648" s="12"/>
+      <c r="B648" s="15"/>
+      <c r="C648" s="15"/>
+      <c r="D648" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="649" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A649" s="12"/>
+      <c r="B649" s="15"/>
+      <c r="C649" s="15"/>
+      <c r="D649" s="7"/>
+    </row>
+    <row r="650" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A650" s="12"/>
+      <c r="B650" s="1"/>
+      <c r="C650" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D650" s="25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="651" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A651" s="12"/>
+      <c r="B651" s="1"/>
+      <c r="C651" s="12"/>
+      <c r="D651" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="652" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A652" s="12"/>
+      <c r="B652" s="1"/>
+      <c r="C652" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D652" s="6"/>
+    </row>
+    <row r="653" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A653" s="12"/>
+      <c r="B653" s="1"/>
+      <c r="C653" s="12"/>
+      <c r="D653" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A654" s="12"/>
+      <c r="B654" s="1"/>
+      <c r="C654" s="12"/>
+      <c r="D654" s="7"/>
+    </row>
+    <row r="655" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A655" s="12"/>
+      <c r="B655" s="1"/>
+      <c r="C655" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D655" s="7"/>
+    </row>
+    <row r="656" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A656" s="12"/>
+      <c r="B656" s="1"/>
+      <c r="C656" s="12"/>
+      <c r="D656" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="657" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A657" s="12"/>
+      <c r="B657" s="1"/>
+      <c r="C657" s="12"/>
+      <c r="D657" s="7"/>
+    </row>
+    <row r="658" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A658" s="12"/>
+      <c r="B658" s="1"/>
+      <c r="C658" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D658" s="10"/>
+    </row>
+    <row r="659" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A659" s="12"/>
+      <c r="B659" s="1"/>
+      <c r="C659" s="12"/>
+      <c r="D659" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A660" s="12"/>
+      <c r="B660" s="1"/>
+      <c r="C660" s="12"/>
+      <c r="D660" s="20"/>
+    </row>
+    <row r="661" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A661" s="12"/>
+      <c r="B661" s="15"/>
+      <c r="C661" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D661" s="6"/>
+    </row>
+    <row r="662" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A662" s="12"/>
+      <c r="B662" s="15"/>
+      <c r="C662" s="15"/>
+      <c r="D662" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="663" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A663" s="12"/>
+      <c r="B663" s="15"/>
+      <c r="C663" s="15"/>
+      <c r="D663" s="7"/>
+    </row>
+    <row r="664" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A664" s="12"/>
+      <c r="B664" s="1"/>
+      <c r="C664" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D664" s="10"/>
+    </row>
+    <row r="665" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A665" s="12"/>
+      <c r="B665" s="1"/>
+      <c r="C665" s="12"/>
+      <c r="D665" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="667" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A667" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="524" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A524" s="28"/>
-    </row>
-    <row r="525" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A525" s="27" t="s">
+    <row r="668" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A668" s="27"/>
+      <c r="C668" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="669" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A669" s="27"/>
+      <c r="D669" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="670" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A670" s="27"/>
+      <c r="D670" s="8"/>
+    </row>
+    <row r="671" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A671" s="27"/>
+      <c r="C671" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D671" s="8"/>
+    </row>
+    <row r="672" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D672" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="674" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A674" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="526" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A526" s="28"/>
-    </row>
-    <row r="527" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A527" s="27" t="s">
+    <row r="675" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A675" s="27"/>
+      <c r="C675" t="s">
+        <v>229</v>
+      </c>
+      <c r="D675" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="676" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A676" s="27"/>
+      <c r="D676" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="677" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A677" s="27"/>
+    </row>
+    <row r="678" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A678" s="27"/>
+      <c r="C678" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="679" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A679" s="27"/>
+      <c r="D679" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="680" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A680" s="27"/>
+    </row>
+    <row r="681" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A681" s="27"/>
+      <c r="C681" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="682" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A682" s="27"/>
+      <c r="D682" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="683" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A683" s="27"/>
+    </row>
+    <row r="684" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A684" s="27"/>
+      <c r="C684" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="685" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A685" s="27"/>
+      <c r="D685" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="686" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A686" s="27"/>
+    </row>
+    <row r="687" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A687" s="27"/>
+      <c r="C687" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="688" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A688" s="27"/>
+      <c r="D688" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A689" s="27"/>
+    </row>
+    <row r="690" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A690" s="27"/>
+      <c r="C690" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A691" s="27"/>
+      <c r="D691" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A692" s="27"/>
+    </row>
+    <row r="693" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A693" s="27"/>
+      <c r="C693" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A694" s="27"/>
+      <c r="D694" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A696" s="27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="528" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A528" s="28"/>
-    </row>
-    <row r="529" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A529" s="27" t="s">
+    <row r="697" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A697" s="27"/>
+      <c r="C697" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A698" s="27"/>
+      <c r="D698" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A699" s="27"/>
+    </row>
+    <row r="700" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A700" s="27"/>
+      <c r="C700" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A701" s="27"/>
+      <c r="D701" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A703" s="27" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="530" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A530" s="28"/>
-    </row>
-    <row r="531" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A531" s="27" t="s">
+    <row r="704" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A704" s="27"/>
+      <c r="C704" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="705" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A705" s="27"/>
+      <c r="D705" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="706" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A706" s="27"/>
+      <c r="C706" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="707" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A707" s="27"/>
+      <c r="D707" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="708" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A708" s="27"/>
+    </row>
+    <row r="709" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A709" s="27"/>
+      <c r="C709" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="710" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A710" s="27"/>
+      <c r="D710" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A712" s="27" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="532" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A532" s="28"/>
-    </row>
-    <row r="533" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A533" s="27" t="s">
+    <row r="713" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A713" s="27"/>
+      <c r="C713" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A714" s="27"/>
+      <c r="D714" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A715" s="27"/>
+      <c r="D715" s="8"/>
+    </row>
+    <row r="716" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A716" s="27"/>
+      <c r="C716" t="s">
+        <v>229</v>
+      </c>
+      <c r="D716" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A717" s="27"/>
+      <c r="D717" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A718" s="27"/>
+    </row>
+    <row r="719" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A719" s="27"/>
+      <c r="C719" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A720" s="27"/>
+      <c r="D720" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A721" s="27"/>
+    </row>
+    <row r="722" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A722" s="27"/>
+      <c r="C722" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A723" s="27"/>
+      <c r="D723" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A724" s="27"/>
+    </row>
+    <row r="725" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A725" s="27"/>
+      <c r="C725" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="726" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A726" s="27"/>
+      <c r="D726" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A727" s="27"/>
+    </row>
+    <row r="728" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A728" s="27"/>
+      <c r="C728" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="729" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A729" s="27"/>
+      <c r="D729" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A730" s="27"/>
+    </row>
+    <row r="731" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A731" s="27"/>
+      <c r="C731" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A732" s="27"/>
+      <c r="D732" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A733" s="27"/>
+    </row>
+    <row r="734" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A734" s="27"/>
+      <c r="C734" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A735" s="27"/>
+      <c r="D735" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A737" s="27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="534" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A534" s="28"/>
-    </row>
-    <row r="535" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A535" s="27" t="s">
+    <row r="738" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A738" s="27"/>
+      <c r="C738" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="739" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A739" s="27"/>
+      <c r="D739" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="740" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A740" s="27"/>
+      <c r="D740" s="8"/>
+    </row>
+    <row r="741" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A741" s="26"/>
+      <c r="C741" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="742" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A742" s="26"/>
+      <c r="C742" s="8"/>
+      <c r="D742" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A743" s="26"/>
+      <c r="C743" s="8"/>
+    </row>
+    <row r="744" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A744" s="26"/>
+      <c r="C744" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="745" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A745" s="26"/>
+      <c r="C745" s="8"/>
+      <c r="D745" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="746" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A746" s="26"/>
+      <c r="C746" s="8"/>
+    </row>
+    <row r="747" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A747" s="26"/>
+      <c r="C747" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="748" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A748" s="26"/>
+      <c r="C748" s="8"/>
+      <c r="D748" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="750" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A750" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="536" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A536" s="28"/>
-    </row>
-    <row r="537" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A537" s="27" t="s">
+    <row r="751" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A751" s="27"/>
+      <c r="C751" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="752" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A752" s="27"/>
+      <c r="D752" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="754" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A754" s="27" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="538" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A538" s="28"/>
-    </row>
-    <row r="539" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A539" s="27" t="s">
+    <row r="755" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A755" s="27"/>
+      <c r="C755" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="756" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A756" s="27"/>
+      <c r="C756" s="8"/>
+      <c r="D756" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="757" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A757" s="27"/>
+      <c r="C757" s="8"/>
+    </row>
+    <row r="758" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A758" s="27"/>
+      <c r="C758" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="759" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A759" s="27"/>
+      <c r="C759" s="8"/>
+      <c r="D759" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="760" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A760" s="27"/>
+      <c r="C760" s="8"/>
+    </row>
+    <row r="761" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A761" s="27"/>
+      <c r="C761" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="762" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A762" s="27"/>
+      <c r="C762" s="8"/>
+      <c r="D762" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="763" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A763" s="27"/>
+      <c r="C763" s="8"/>
+    </row>
+    <row r="764" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A764" s="27"/>
+      <c r="C764" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="765" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A765" s="27"/>
+      <c r="C765" s="8"/>
+      <c r="D765" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A766" s="27"/>
+      <c r="C766" s="8"/>
+    </row>
+    <row r="767" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A767" s="27"/>
+      <c r="C767" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A768" s="27"/>
+      <c r="D768" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A769" s="27"/>
+    </row>
+    <row r="770" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A770" s="27"/>
+      <c r="C770" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A771" s="27"/>
+      <c r="D771" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A772" s="27"/>
+    </row>
+    <row r="773" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A773" s="27"/>
+      <c r="C773" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A774" s="27"/>
+      <c r="D774" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A775" s="27"/>
+    </row>
+    <row r="776" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A776" s="27"/>
+      <c r="C776" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A777" s="27"/>
+      <c r="D777" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A779" s="27" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="540" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A540" s="28"/>
-    </row>
-    <row r="541" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A541" s="27" t="s">
+    <row r="780" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A780" s="27"/>
+      <c r="C780" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A781" s="27"/>
+      <c r="D781" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A782" s="27"/>
+      <c r="D782" s="8"/>
+    </row>
+    <row r="783" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A783" s="27"/>
+      <c r="C783" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D783" s="8"/>
+    </row>
+    <row r="784" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A784" s="27"/>
+      <c r="D784" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="785" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A785" s="27"/>
+      <c r="D785" s="8"/>
+    </row>
+    <row r="786" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A786" s="27"/>
+      <c r="C786" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D786" s="8"/>
+    </row>
+    <row r="787" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A787" s="27"/>
+      <c r="D787" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="788" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A788" s="27"/>
+      <c r="D788" s="8"/>
+    </row>
+    <row r="789" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A789" s="27"/>
+      <c r="C789" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D789" s="25" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="790" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A790" s="27"/>
+      <c r="D790" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="791" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A791" s="27"/>
+      <c r="D791" s="8"/>
+    </row>
+    <row r="792" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A792" s="27"/>
+      <c r="C792" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D792" s="25" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="793" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A793" s="27"/>
+      <c r="D793" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="794" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A794" s="27"/>
+      <c r="D794" s="8"/>
+    </row>
+    <row r="795" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A795" s="27"/>
+      <c r="C795" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D795" s="8"/>
+    </row>
+    <row r="796" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A796" s="27"/>
+      <c r="C796" s="8"/>
+      <c r="D796" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="797" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A797" s="27"/>
+      <c r="C797" s="8"/>
+      <c r="D797" s="8"/>
+    </row>
+    <row r="798" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A798" s="27"/>
+      <c r="C798" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D798" s="8"/>
+    </row>
+    <row r="799" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A799" s="27"/>
+      <c r="C799" s="8"/>
+      <c r="D799" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="800" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A800" s="27"/>
+      <c r="C800" s="8"/>
+      <c r="D800" s="8"/>
+    </row>
+    <row r="801" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A801" s="27"/>
+      <c r="C801" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D801" s="8"/>
+    </row>
+    <row r="802" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A802" s="27"/>
+      <c r="C802" s="8"/>
+      <c r="D802" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="804" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A804" s="27" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="542" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A542" s="28"/>
-    </row>
-    <row r="543" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A543" s="27" t="s">
+    <row r="805" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A805" s="27"/>
+      <c r="C805" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="806" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A806" s="27"/>
+      <c r="D806" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="807" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A807" s="27"/>
+    </row>
+    <row r="808" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A808" s="27"/>
+      <c r="C808" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="809" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A809" s="27"/>
+      <c r="D809" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="810" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A810" s="27"/>
+    </row>
+    <row r="811" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A811" s="27"/>
+      <c r="C811" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="812" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A812" s="27"/>
+      <c r="D812" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="813" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A813" s="27"/>
+      <c r="D813" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="815" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A815" s="27" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="544" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A544" s="28"/>
-    </row>
-    <row r="545" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A545" s="27" t="s">
+    <row r="816" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A816" s="27"/>
+      <c r="C816" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="817" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A817" s="27"/>
+      <c r="D817" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="818" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A818" s="27"/>
+      <c r="D818" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="819" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A819" s="27"/>
+      <c r="D819" s="8"/>
+    </row>
+    <row r="820" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A820" s="27"/>
+      <c r="C820" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="D820" s="8"/>
+    </row>
+    <row r="821" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D821" s="23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="822" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D822" s="23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="823" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D823" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="824" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D824" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="825" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D825" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="826" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D826" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="827" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D827" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="828" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D828" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="829" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D829" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="830" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D830" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="831" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D831" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="833" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A833" s="27" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="834" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C834" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="835" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D835" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="837" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C837" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="838" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D838" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="840" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C840" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="841" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D841" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="843" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C843" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="844" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D844" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="846" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C846" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="847" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D847" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="849" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C849" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="850" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D850" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="852" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C852" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="853" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D853" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="855" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C855" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="856" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D856" s="8" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4980,6 +7017,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="1564dcde-57fb-47ba-809c-59eaaf97e9ec" xsi:nil="true"/>
@@ -4988,15 +7034,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5237,20 +7274,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD654986-07A1-4359-ADBD-FDF37DFE15EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE1CDC5F-8AA7-4CFE-960A-82DBC0D5EA69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1564dcde-57fb-47ba-809c-59eaaf97e9ec"/>
     <ds:schemaRef ds:uri="d2f27c1e-3f69-4f81-a6fe-887d5ff4e0df"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD654986-07A1-4359-ADBD-FDF37DFE15EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>